<commit_message>
updated KARMEN docs based on updated Dataschema
</commit_message>
<xml_diff>
--- a/Tracy/DPE_KARMEN_TRACY.xlsx
+++ b/Tracy/DPE_KARMEN_TRACY.xlsx
@@ -1017,7 +1017,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Age at diagnosis of CVD</t>
+          <t>Age at diagnosis of CVD [years]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Age at diagnosis of angina pectoris</t>
+          <t>Age at diagnosis of angina pectoris [years]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Age at diagnosis of myocardial infarction</t>
+          <t>Age at diagnosis of myocardial infarction [years]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Age at diagnosis of stroke</t>
+          <t>Age at diagnosis of stroke [years]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Age at diagnosis of cerebral infarction (ischaemic stroke)</t>
+          <t>Age at diagnosis of cerebral infarction (ischaemic stroke) [years]</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Age at diagnosis of haemorrhagic stroke</t>
+          <t>Age at diagnosis of haemorrhagic stroke [years]</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Age at diagnosis of essential hypertension</t>
+          <t>Age at diagnosis of essential hypertension [years]</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Age at diagnosis of heart failure</t>
+          <t>Age at diagnosis of heart failure [years]</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Age at diagnosis of diabetes mellitus type 2</t>
+          <t>Age at diagnosis of diabetes mellitus type 2 [years]</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Age at diagnosis of cancer</t>
+          <t>Age at diagnosis of cancer [years]</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Age at time of death</t>
+          <t>Age at time of death [years]</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">

</xml_diff>

<commit_message>
DPE_KARMEN_TRACY -> col_id to id and filled "input_variables" where blank
</commit_message>
<xml_diff>
--- a/Tracy/DPE_KARMEN_TRACY.xlsx
+++ b/Tracy/DPE_KARMEN_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Tracy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8776A090-EC9C-4E44-8A84-2AD04460E32E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500D4F5F-872C-413E-8604-A19252FE59D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="162">
   <si>
     <t>index</t>
   </si>
@@ -445,9 +445,6 @@
     <t>Age at end of follow-up</t>
   </si>
   <si>
-    <t>col_id</t>
-  </si>
-  <si>
     <t>id_creation</t>
   </si>
   <si>
@@ -506,6 +503,9 @@
   </si>
   <si>
     <t>due to inclusion criteria, all participants were healthy at time of reruitment without a history of cancer; new variable could be created coded =0 for all participants</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,6 +620,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -961,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,22 +1027,22 @@
         <v>13</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>142</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1054,20 +1056,20 @@
         <v>13</v>
       </c>
       <c r="F3" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1081,20 +1083,20 @@
         <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1107,7 +1109,9 @@
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>113</v>
       </c>
@@ -1134,7 +1138,9 @@
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>113</v>
       </c>
@@ -1161,7 +1167,9 @@
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>113</v>
       </c>
@@ -1217,7 +1225,9 @@
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>113</v>
       </c>
@@ -1225,13 +1235,13 @@
         <v>113</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>156</v>
+        <v>153</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1245,19 +1255,19 @@
         <v>13</v>
       </c>
       <c r="F10" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H10" s="8">
         <v>0</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
+        <v>154</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -1270,19 +1280,19 @@
         <v>17</v>
       </c>
       <c r="F11" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H11" s="8">
         <v>0</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>111</v>
@@ -1299,19 +1309,19 @@
         <v>13</v>
       </c>
       <c r="F12" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H12" s="8">
         <v>0</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>111</v>
@@ -1328,19 +1338,19 @@
         <v>13</v>
       </c>
       <c r="F13" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H13" s="8">
         <v>0</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>111</v>
@@ -1356,7 +1366,9 @@
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G14" s="2" t="s">
         <v>113</v>
       </c>
@@ -1364,10 +1376,10 @@
         <v>113</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>111</v>
@@ -1384,17 +1396,17 @@
         <v>13</v>
       </c>
       <c r="F15" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>150</v>
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>111</v>
@@ -1411,17 +1423,17 @@
         <v>13</v>
       </c>
       <c r="F16" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H16" s="8">
         <v>0</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>111</v>
@@ -1438,19 +1450,19 @@
         <v>13</v>
       </c>
       <c r="F17" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H17" s="8">
         <v>0</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>111</v>
@@ -1466,7 +1478,9 @@
       <c r="D18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G18" s="2" t="s">
         <v>113</v>
       </c>
@@ -1474,10 +1488,10 @@
         <v>113</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>111</v>
@@ -1493,7 +1507,9 @@
       <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G19" s="2" t="s">
         <v>113</v>
       </c>
@@ -1519,17 +1535,17 @@
         <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H20" s="8">
         <v>0</v>
       </c>
       <c r="I20" s="15"/>
       <c r="J20" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>111</v>
@@ -1546,19 +1562,19 @@
         <v>13</v>
       </c>
       <c r="F21" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H21" s="8">
         <v>0</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>111</v>
@@ -1575,19 +1591,19 @@
         <v>13</v>
       </c>
       <c r="F22" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H22" s="8">
         <v>0</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>111</v>
@@ -1604,19 +1620,19 @@
         <v>13</v>
       </c>
       <c r="F23" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H23" s="8">
         <v>0</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>111</v>
@@ -1632,18 +1648,20 @@
       <c r="D24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>111</v>
@@ -1659,9 +1677,11 @@
       <c r="D25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G25" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>113</v>
@@ -1686,9 +1706,11 @@
       <c r="D26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G26" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>113</v>
@@ -1713,9 +1735,11 @@
       <c r="D27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G27" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>113</v>
@@ -1740,9 +1764,11 @@
       <c r="D28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G28" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>113</v>
@@ -1767,9 +1793,11 @@
       <c r="D29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G29" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>113</v>
@@ -1794,9 +1822,11 @@
       <c r="D30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G30" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>113</v>
@@ -1805,7 +1835,7 @@
         <v>114</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>114</v>
@@ -1821,9 +1851,11 @@
       <c r="D31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G31" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>113</v>
@@ -1848,9 +1880,11 @@
       <c r="D32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G32" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>113</v>
@@ -1875,9 +1909,11 @@
       <c r="D33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="17" t="s">
+        <v>150</v>
+      </c>
       <c r="G33" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>113</v>
@@ -1903,10 +1939,10 @@
         <v>13</v>
       </c>
       <c r="F34" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H34" s="8">
         <v>0</v>
@@ -1932,19 +1968,19 @@
         <v>13</v>
       </c>
       <c r="F35" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G35" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="H35" s="8">
         <v>0</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>111</v>
@@ -1960,7 +1996,9 @@
       <c r="D36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G36" s="2" t="s">
         <v>113</v>
       </c>
@@ -1968,10 +2006,10 @@
         <v>113</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>111</v>
@@ -1987,7 +2025,9 @@
       <c r="D37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G37" s="2" t="s">
         <v>113</v>
       </c>
@@ -2014,7 +2054,9 @@
       <c r="D38" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G38" s="2" t="s">
         <v>113</v>
       </c>
@@ -2041,7 +2083,9 @@
       <c r="D39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="2"/>
+      <c r="F39" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G39" s="2" t="s">
         <v>113</v>
       </c>
@@ -2068,7 +2112,9 @@
       <c r="D40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G40" s="2" t="s">
         <v>113</v>
       </c>
@@ -2095,7 +2141,9 @@
       <c r="D41" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G41" s="2" t="s">
         <v>113</v>
       </c>
@@ -2122,7 +2170,9 @@
       <c r="D42" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G42" s="2" t="s">
         <v>113</v>
       </c>
@@ -2149,7 +2199,9 @@
       <c r="D43" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G43" s="2" t="s">
         <v>113</v>
       </c>
@@ -2176,7 +2228,9 @@
       <c r="D44" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="2"/>
+      <c r="F44" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G44" s="2" t="s">
         <v>113</v>
       </c>
@@ -2203,7 +2257,9 @@
       <c r="D45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G45" s="2" t="s">
         <v>113</v>
       </c>
@@ -2230,7 +2286,9 @@
       <c r="D46" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="2"/>
+      <c r="F46" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G46" s="2" t="s">
         <v>113</v>
       </c>
@@ -2257,7 +2315,9 @@
       <c r="D47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F47" s="2"/>
+      <c r="F47" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G47" s="2" t="s">
         <v>113</v>
       </c>
@@ -2284,7 +2344,9 @@
       <c r="D48" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="2"/>
+      <c r="F48" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G48" s="2" t="s">
         <v>113</v>
       </c>
@@ -2311,7 +2373,9 @@
       <c r="D49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="2"/>
+      <c r="F49" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G49" s="2" t="s">
         <v>113</v>
       </c>
@@ -2338,7 +2402,9 @@
       <c r="D50" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G50" s="2" t="s">
         <v>113</v>
       </c>
@@ -2365,7 +2431,9 @@
       <c r="D51" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="2"/>
+      <c r="F51" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G51" s="2" t="s">
         <v>113</v>
       </c>
@@ -2392,7 +2460,9 @@
       <c r="D52" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G52" s="2" t="s">
         <v>113</v>
       </c>
@@ -2419,7 +2489,9 @@
       <c r="D53" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="F53" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G53" s="2" t="s">
         <v>113</v>
       </c>
@@ -2446,7 +2518,9 @@
       <c r="D54" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G54" s="2" t="s">
         <v>113</v>
       </c>
@@ -2473,7 +2547,9 @@
       <c r="D55" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F55" s="2"/>
+      <c r="F55" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G55" s="2" t="s">
         <v>113</v>
       </c>
@@ -2500,7 +2576,9 @@
       <c r="D56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G56" s="2" t="s">
         <v>113</v>
       </c>
@@ -2527,7 +2605,9 @@
       <c r="D57" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G57" s="2" t="s">
         <v>113</v>
       </c>
@@ -2554,7 +2634,9 @@
       <c r="D58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G58" s="2" t="s">
         <v>113</v>
       </c>
@@ -2581,7 +2663,9 @@
       <c r="D59" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F59" s="2"/>
+      <c r="F59" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G59" s="2" t="s">
         <v>113</v>
       </c>
@@ -2608,7 +2692,9 @@
       <c r="D60" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="2"/>
+      <c r="F60" s="17" t="s">
+        <v>113</v>
+      </c>
       <c r="G60" s="2" t="s">
         <v>113</v>
       </c>
@@ -2636,20 +2722,22 @@
         <v>17</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="I61" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="J61" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="K61" s="8" t="s">
-        <v>153</v>
+        <v>113</v>
+      </c>
+      <c r="K61" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
filled out "input_variables" where blank and col_id to id
</commit_message>
<xml_diff>
--- a/Tracy/DPE_KARMEN_TRACY.xlsx
+++ b/Tracy/DPE_KARMEN_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Tracy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A386BF7-A6EA-4888-993B-8FD48F6A3689}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461F6497-02EE-4A9C-A988-06C845A7F7A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="159">
   <si>
     <t>index</t>
   </si>
@@ -424,9 +424,6 @@
     <t>Age at end of follow-up [years]</t>
   </si>
   <si>
-    <t>col_id</t>
-  </si>
-  <si>
     <t>id_creation</t>
   </si>
   <si>
@@ -497,6 +494,9 @@
   </si>
   <si>
     <t xml:space="preserve">impossible </t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,22 +987,22 @@
         <v>13</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1016,20 +1016,20 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1043,20 +1043,20 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1069,21 +1069,23 @@
       <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G5" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1097,22 +1099,22 @@
         <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1125,21 +1127,23 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G7" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1152,20 +1156,23 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G8" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1178,20 +1185,23 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G9" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1204,18 +1214,21 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G10" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1228,18 +1241,21 @@
       <c r="D11" t="s">
         <v>18</v>
       </c>
+      <c r="F11" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G11" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1252,18 +1268,21 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
+      <c r="F12" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G12" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1276,18 +1295,21 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G13" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1300,18 +1322,21 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
+      <c r="F14" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G14" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1325,20 +1350,20 @@
         <v>13</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1352,22 +1377,22 @@
         <v>13</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H16" s="3">
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="90" x14ac:dyDescent="0.25">
@@ -1381,22 +1406,22 @@
         <v>13</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H17" s="3">
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1409,19 +1434,21 @@
       <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G18" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1434,19 +1461,21 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G19" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1460,22 +1489,22 @@
         <v>13</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H20" s="3">
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1489,22 +1518,22 @@
         <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H21" s="3">
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1518,22 +1547,22 @@
         <v>13</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1547,22 +1576,22 @@
         <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1575,21 +1604,23 @@
       <c r="D24" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
@@ -1602,21 +1633,23 @@
       <c r="D25" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G25" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
@@ -1629,21 +1662,23 @@
       <c r="D26" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G26" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1656,21 +1691,23 @@
       <c r="D27" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G27" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
@@ -1683,21 +1720,23 @@
       <c r="D28" t="s">
         <v>13</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G28" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
@@ -1710,21 +1749,23 @@
       <c r="D29" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G29" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
@@ -1737,21 +1778,23 @@
       <c r="D30" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G30" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1764,21 +1807,23 @@
       <c r="D31" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G31" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
@@ -1791,21 +1836,23 @@
       <c r="D32" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G32" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
@@ -1818,21 +1865,23 @@
       <c r="D33" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G33" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1846,22 +1895,22 @@
         <v>13</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H34" s="3">
         <v>0</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1875,22 +1924,22 @@
         <v>13</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="H35" s="3">
         <v>0</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -1903,21 +1952,23 @@
       <c r="D36" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G36" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -1930,21 +1981,23 @@
       <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -1957,21 +2010,23 @@
       <c r="D38" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="3"/>
+      <c r="F38" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G38" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
@@ -1984,21 +2039,23 @@
       <c r="D39" t="s">
         <v>18</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G39" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
@@ -2011,21 +2068,23 @@
       <c r="D40" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G40" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
@@ -2038,21 +2097,23 @@
       <c r="D41" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G41" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
@@ -2065,21 +2126,23 @@
       <c r="D42" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G42" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
@@ -2092,21 +2155,23 @@
       <c r="D43" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G43" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
@@ -2119,21 +2184,23 @@
       <c r="D44" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G44" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
@@ -2146,21 +2213,23 @@
       <c r="D45" t="s">
         <v>18</v>
       </c>
-      <c r="F45" s="3"/>
+      <c r="F45" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G45" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
@@ -2173,21 +2242,23 @@
       <c r="D46" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="3"/>
+      <c r="F46" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G46" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
@@ -2200,21 +2271,23 @@
       <c r="D47" t="s">
         <v>18</v>
       </c>
-      <c r="F47" s="3"/>
+      <c r="F47" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G47" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
@@ -2227,21 +2300,23 @@
       <c r="D48" t="s">
         <v>13</v>
       </c>
-      <c r="F48" s="3"/>
+      <c r="F48" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G48" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K48" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -2254,21 +2329,23 @@
       <c r="D49" t="s">
         <v>18</v>
       </c>
-      <c r="F49" s="3"/>
+      <c r="F49" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G49" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
@@ -2281,21 +2358,23 @@
       <c r="D50" t="s">
         <v>13</v>
       </c>
-      <c r="F50" s="3"/>
+      <c r="F50" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G50" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
@@ -2308,21 +2387,23 @@
       <c r="D51" t="s">
         <v>18</v>
       </c>
-      <c r="F51" s="3"/>
+      <c r="F51" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G51" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
@@ -2335,21 +2416,23 @@
       <c r="D52" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="3"/>
+      <c r="F52" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G52" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
@@ -2362,21 +2445,23 @@
       <c r="D53" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G53" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
@@ -2389,21 +2474,23 @@
       <c r="D54" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
@@ -2416,21 +2503,23 @@
       <c r="D55" t="s">
         <v>121</v>
       </c>
-      <c r="F55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G55" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
@@ -2443,21 +2532,23 @@
       <c r="D56" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G56" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
@@ -2470,21 +2561,23 @@
       <c r="D57" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="3"/>
+      <c r="F57" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G57" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
@@ -2497,21 +2590,23 @@
       <c r="D58" t="s">
         <v>18</v>
       </c>
-      <c r="F58" s="3"/>
+      <c r="F58" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G58" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
@@ -2524,21 +2619,23 @@
       <c r="D59" t="s">
         <v>13</v>
       </c>
-      <c r="F59" s="3"/>
+      <c r="F59" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G59" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
@@ -2551,21 +2648,23 @@
       <c r="D60" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="3"/>
+      <c r="F60" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G60" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K60" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
@@ -2578,21 +2677,23 @@
       <c r="D61" t="s">
         <v>18</v>
       </c>
-      <c r="F61" s="3"/>
+      <c r="F61" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G61" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TOT_PA_QX harmo comment MET-min/week from MET-min/Wo
</commit_message>
<xml_diff>
--- a/Tracy/DPE_KARMEN_TRACY.xlsx
+++ b/Tracy/DPE_KARMEN_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Tracy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461F6497-02EE-4A9C-A988-06C845A7F7A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4171F97-EEBB-4261-BDEE-BAE6437E9EC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,9 +457,6 @@
     <t>(IPAQ_MET_Total*60)/7</t>
   </si>
   <si>
-    <t>MET-min/Wo</t>
-  </si>
-  <si>
     <t>compatible</t>
   </si>
   <si>
@@ -497,6 +494,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>MET-min/week</t>
   </si>
 </sst>
 </file>
@@ -924,7 +924,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,7 +987,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>134</v>
@@ -1108,13 +1108,13 @@
         <v>144</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1350,20 +1350,20 @@
         <v>13</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1377,22 +1377,22 @@
         <v>13</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="H16" s="3">
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="90" x14ac:dyDescent="0.25">
@@ -1406,22 +1406,22 @@
         <v>13</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="H17" s="3">
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1489,22 +1489,22 @@
         <v>13</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="H20" s="3">
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1518,22 +1518,22 @@
         <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="H21" s="3">
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1547,22 +1547,22 @@
         <v>13</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1576,22 +1576,22 @@
         <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -1608,7 +1608,7 @@
         <v>140</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>140</v>
@@ -1637,7 +1637,7 @@
         <v>140</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>140</v>
@@ -1666,7 +1666,7 @@
         <v>140</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>140</v>
@@ -1695,7 +1695,7 @@
         <v>140</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>140</v>
@@ -1724,7 +1724,7 @@
         <v>140</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>140</v>
@@ -1753,7 +1753,7 @@
         <v>140</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>140</v>
@@ -1762,7 +1762,7 @@
         <v>141</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>141</v>
@@ -1782,7 +1782,7 @@
         <v>140</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>140</v>
@@ -1811,7 +1811,7 @@
         <v>140</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>140</v>
@@ -1840,7 +1840,7 @@
         <v>140</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>140</v>
@@ -1869,7 +1869,7 @@
         <v>140</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>140</v>
@@ -1895,22 +1895,22 @@
         <v>13</v>
       </c>
       <c r="F34" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="H34" s="3">
         <v>0</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="2:11" ht="120" x14ac:dyDescent="0.25">
@@ -1924,22 +1924,22 @@
         <v>13</v>
       </c>
       <c r="F35" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="H35" s="3">
         <v>0</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">

</xml_diff>